<commit_message>
Added PersonStateFingerprintIdentification to SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Consolidation_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Consolidation_IEPD/documentation/mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Criminal_History_Consolidation_Reporting_Service/artifacts/service_model/information_model/Criminal_History_Consolidation_IEPD/documentation/mapping.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="26925" windowHeight="10365"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="26920" windowHeight="10360"/>
   </bookViews>
   <sheets>
     <sheet name="Request" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Business</t>
   </si>
@@ -65,13 +70,22 @@
   </si>
   <si>
     <t>/CHcr-doc:CriminalHistoryConsolidationReport/nc:Person/CHcr-ext:PostConsolidationIdentifiers/j:PersonFBIIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Person State Fingerprint ID</t>
+  </si>
+  <si>
+    <t>An identification of a person based on a Fingerprint ID.</t>
+  </si>
+  <si>
+    <t>/CHcr-doc:CriminalHistoryConsolidationReport/nc:Person/CHcr-ext:PostConsolidationIdentifiers/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +262,22 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -614,7 +644,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -657,6 +687,8 @@
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -667,12 +699,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -693,6 +719,12 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -700,7 +732,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -729,11 +761,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1041,50 +1075,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="126.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="62.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="32.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="126.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" ht="45" hidden="1" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="45" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="13"/>
-      <c r="C2" s="7"/>
+      <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" s="2" customFormat="1" ht="18">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1093,56 +1127,67 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:3" ht="28">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1152,6 +1197,11 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>